<commit_message>
Update Number of large herbivores in the Oostvaardersplassen 1985 - 2015.xlsx
</commit_message>
<xml_diff>
--- a/Data/Number of large herbivores in the Oostvaardersplassen 1985 - 2015.xlsx
+++ b/Data/Number of large herbivores in the Oostvaardersplassen 1985 - 2015.xlsx
@@ -1,22 +1,36 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21029"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Justin\Documents\GitHub\ApplicationDevelopment\Data\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E59AD0BB-374F-41F6-8095-B838ECDC2BB5}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="45" windowWidth="20115" windowHeight="7995"/>
+    <workbookView xWindow="240" yWindow="48" windowWidth="20112" windowHeight="7992" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
     <sheet name="Blad2" sheetId="2" r:id="rId2"/>
     <sheet name="Blad3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="16">
   <si>
     <t>Heck cattle</t>
   </si>
@@ -44,11 +58,32 @@
   <si>
     <t>Total</t>
   </si>
+  <si>
+    <t>death red deer:</t>
+  </si>
+  <si>
+    <t>instantaneous dr</t>
+  </si>
+  <si>
+    <t>birth red deer:</t>
+  </si>
+  <si>
+    <t>instantaneous birth rate:</t>
+  </si>
+  <si>
+    <t>red deer :</t>
+  </si>
+  <si>
+    <t xml:space="preserve">r = </t>
+  </si>
+  <si>
+    <t>don"t count the last years bc of the capacity and something obviously happened there.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="11">
     <font>
       <sz val="10"/>
@@ -169,16 +204,16 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="10">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Standaard 2" xfId="2"/>
-    <cellStyle name="Standaard 2 2" xfId="5"/>
-    <cellStyle name="Standaard 3" xfId="1"/>
-    <cellStyle name="Standaard 3 2" xfId="3"/>
-    <cellStyle name="Standaard 4" xfId="6"/>
-    <cellStyle name="Standaard 5" xfId="7"/>
-    <cellStyle name="Standaard 6" xfId="9"/>
-    <cellStyle name="Standaard 7" xfId="8"/>
-    <cellStyle name="Standaard 8" xfId="4"/>
+    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
+    <cellStyle name="Standaard 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="Standaard 2 2" xfId="5" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
+    <cellStyle name="Standaard 3" xfId="1" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
+    <cellStyle name="Standaard 3 2" xfId="3" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
+    <cellStyle name="Standaard 4" xfId="6" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
+    <cellStyle name="Standaard 5" xfId="7" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
+    <cellStyle name="Standaard 6" xfId="9" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
+    <cellStyle name="Standaard 7" xfId="8" xr:uid="{00000000-0005-0000-0000-000008000000}"/>
+    <cellStyle name="Standaard 8" xfId="4" xr:uid="{00000000-0005-0000-0000-000009000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -186,12 +221,15 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Kantoorthema">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -233,7 +271,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -266,9 +304,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -301,6 +356,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -476,38 +548,39 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q38"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:W43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" topLeftCell="E15" workbookViewId="0">
+      <selection activeCell="T37" sqref="T37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultRowHeight="13.2"/>
   <cols>
     <col min="1" max="1" width="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="36.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="36.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="5.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.5703125" customWidth="1"/>
-    <col min="9" max="9" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.5546875" customWidth="1"/>
+    <col min="9" max="9" width="12.33203125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="9" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="5.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="5.109375" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="5" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.33203125" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="9" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="5.140625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="5.109375" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="9.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="15" customFormat="1">
+    <row r="1" spans="1:23" s="15" customFormat="1">
       <c r="A1" s="14" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:17" s="12" customFormat="1" ht="15">
+    <row r="3" spans="1:23" s="12" customFormat="1" ht="14.4">
       <c r="B3" s="13" t="s">
         <v>5</v>
       </c>
@@ -519,7 +592,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:17" s="12" customFormat="1" ht="15">
+    <row r="5" spans="1:23" s="12" customFormat="1" ht="14.4">
       <c r="A5" s="16" t="s">
         <v>7</v>
       </c>
@@ -566,7 +639,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:17" ht="15">
+    <row r="6" spans="1:23" ht="14.4">
       <c r="A6" s="2">
         <v>1983</v>
       </c>
@@ -598,7 +671,7 @@
       <c r="O6" s="9"/>
       <c r="P6" s="9"/>
     </row>
-    <row r="7" spans="1:17" ht="15">
+    <row r="7" spans="1:23" ht="14.4">
       <c r="A7" s="2">
         <v>1984</v>
       </c>
@@ -638,7 +711,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:17" ht="15">
+    <row r="8" spans="1:23" ht="14.4">
       <c r="A8" s="2">
         <v>1985</v>
       </c>
@@ -682,7 +755,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:17" ht="15">
+    <row r="9" spans="1:23" ht="14.4">
       <c r="A9" s="2">
         <v>1986</v>
       </c>
@@ -726,7 +799,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:17" ht="15">
+    <row r="10" spans="1:23" ht="14.4">
       <c r="A10" s="2">
         <v>1987</v>
       </c>
@@ -770,7 +843,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="11" spans="1:17" ht="15">
+    <row r="11" spans="1:23" ht="14.4">
       <c r="A11" s="2">
         <v>1988</v>
       </c>
@@ -814,7 +887,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="12" spans="1:17" ht="15">
+    <row r="12" spans="1:23" ht="14.4">
       <c r="A12" s="2">
         <v>1989</v>
       </c>
@@ -858,7 +931,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="13" spans="1:17" ht="15">
+    <row r="13" spans="1:23" ht="14.4">
       <c r="A13" s="2">
         <v>1990</v>
       </c>
@@ -902,7 +975,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="14" spans="1:17" ht="15">
+    <row r="14" spans="1:23" ht="14.4">
       <c r="A14" s="2">
         <v>1991</v>
       </c>
@@ -946,7 +1019,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="15" spans="1:17" ht="15">
+    <row r="15" spans="1:23" ht="14.4">
       <c r="A15" s="2">
         <v>1992</v>
       </c>
@@ -995,8 +1068,22 @@
         <f t="shared" si="2"/>
         <v>100</v>
       </c>
-    </row>
-    <row r="16" spans="1:17" ht="15">
+      <c r="S15" t="s">
+        <v>9</v>
+      </c>
+      <c r="T15">
+        <f>J15/D15</f>
+        <v>0.1111111111111111</v>
+      </c>
+      <c r="V15" t="s">
+        <v>11</v>
+      </c>
+      <c r="W15">
+        <f>P15/D15</f>
+        <v>0.44444444444444442</v>
+      </c>
+    </row>
+    <row r="16" spans="1:23" ht="14.4">
       <c r="A16" s="2">
         <v>1993</v>
       </c>
@@ -1045,8 +1132,16 @@
         <f t="shared" si="2"/>
         <v>140</v>
       </c>
-    </row>
-    <row r="17" spans="1:17" ht="15">
+      <c r="T16">
+        <f>J16/D16</f>
+        <v>7.1428571428571425E-2</v>
+      </c>
+      <c r="W16">
+        <f>P16/D16</f>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:23" ht="14.4">
       <c r="A17" s="2">
         <v>1994</v>
       </c>
@@ -1095,8 +1190,16 @@
         <f t="shared" si="2"/>
         <v>160</v>
       </c>
-    </row>
-    <row r="18" spans="1:17" ht="15">
+      <c r="T17">
+        <f>J17/D17</f>
+        <v>0</v>
+      </c>
+      <c r="W17">
+        <f>P17/D17</f>
+        <v>0.35</v>
+      </c>
+    </row>
+    <row r="18" spans="1:23" ht="14.4">
       <c r="A18" s="2">
         <v>1995</v>
       </c>
@@ -1145,8 +1248,16 @@
         <f t="shared" si="2"/>
         <v>160</v>
       </c>
-    </row>
-    <row r="19" spans="1:17" ht="15">
+      <c r="T18">
+        <f>J18/D18</f>
+        <v>3.5714285714285712E-2</v>
+      </c>
+      <c r="W18">
+        <f>P18/D18</f>
+        <v>0.35714285714285715</v>
+      </c>
+    </row>
+    <row r="19" spans="1:23" ht="14.4">
       <c r="A19" s="2">
         <v>1996</v>
       </c>
@@ -1195,8 +1306,16 @@
         <f t="shared" si="2"/>
         <v>200</v>
       </c>
-    </row>
-    <row r="20" spans="1:17" ht="15">
+      <c r="T19">
+        <f>J19/D19</f>
+        <v>2.7777777777777776E-2</v>
+      </c>
+      <c r="W19">
+        <f>P19/D19</f>
+        <v>0.3611111111111111</v>
+      </c>
+    </row>
+    <row r="20" spans="1:23" ht="14.4">
       <c r="A20" s="2">
         <v>1997</v>
       </c>
@@ -1245,8 +1364,16 @@
         <f t="shared" si="2"/>
         <v>260</v>
       </c>
-    </row>
-    <row r="21" spans="1:17" ht="15">
+      <c r="T20">
+        <f>J20/D20</f>
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="W20">
+        <f>P20/D20</f>
+        <v>0.3125</v>
+      </c>
+    </row>
+    <row r="21" spans="1:23" ht="14.4">
       <c r="A21" s="2">
         <v>1998</v>
       </c>
@@ -1295,8 +1422,16 @@
         <f t="shared" si="2"/>
         <v>270</v>
       </c>
-    </row>
-    <row r="22" spans="1:17" ht="15">
+      <c r="T21">
+        <f>J21/D21</f>
+        <v>0</v>
+      </c>
+      <c r="W21">
+        <f>P21/D21</f>
+        <v>0.26666666666666666</v>
+      </c>
+    </row>
+    <row r="22" spans="1:23" ht="14.4">
       <c r="A22" s="2">
         <v>1999</v>
       </c>
@@ -1345,8 +1480,16 @@
         <f t="shared" si="2"/>
         <v>320</v>
       </c>
-    </row>
-    <row r="23" spans="1:17" ht="15">
+      <c r="T22">
+        <f>J22/D22</f>
+        <v>3.9473684210526314E-2</v>
+      </c>
+      <c r="W22">
+        <f>P22/D22</f>
+        <v>0.26315789473684209</v>
+      </c>
+    </row>
+    <row r="23" spans="1:23" ht="14.4">
       <c r="A23" s="2">
         <v>2000</v>
       </c>
@@ -1395,8 +1538,16 @@
         <f t="shared" si="2"/>
         <v>380</v>
       </c>
-    </row>
-    <row r="24" spans="1:17" ht="15">
+      <c r="T23">
+        <f>J23/D23</f>
+        <v>3.2608695652173912E-2</v>
+      </c>
+      <c r="W23">
+        <f>P23/D23</f>
+        <v>0.31521739130434784</v>
+      </c>
+    </row>
+    <row r="24" spans="1:23" ht="14.4">
       <c r="A24" s="2">
         <v>2001</v>
       </c>
@@ -1445,8 +1596,16 @@
         <f t="shared" si="2"/>
         <v>480</v>
       </c>
-    </row>
-    <row r="25" spans="1:17" ht="15">
+      <c r="T24">
+        <f>J24/D24</f>
+        <v>4.2372881355932202E-2</v>
+      </c>
+      <c r="W24">
+        <f>P24/D24</f>
+        <v>0.33898305084745761</v>
+      </c>
+    </row>
+    <row r="25" spans="1:23" ht="14.4">
       <c r="A25" s="2">
         <v>2002</v>
       </c>
@@ -1495,8 +1654,16 @@
         <f t="shared" si="2"/>
         <v>565</v>
       </c>
-    </row>
-    <row r="26" spans="1:17" ht="15">
+      <c r="T25">
+        <f>J25/D25</f>
+        <v>3.2467532467532464E-2</v>
+      </c>
+      <c r="W25">
+        <f>P25/D25</f>
+        <v>0.35064935064935066</v>
+      </c>
+    </row>
+    <row r="26" spans="1:23" ht="14.4">
       <c r="A26" s="2">
         <v>2003</v>
       </c>
@@ -1545,8 +1712,16 @@
         <f t="shared" si="2"/>
         <v>610</v>
       </c>
-    </row>
-    <row r="27" spans="1:17" ht="15">
+      <c r="T26">
+        <f>J26/D26</f>
+        <v>0.13500000000000001</v>
+      </c>
+      <c r="W26">
+        <f>P26/D26</f>
+        <v>0.28000000000000003</v>
+      </c>
+    </row>
+    <row r="27" spans="1:23" ht="14.4">
       <c r="A27" s="2">
         <v>2004</v>
       </c>
@@ -1595,8 +1770,16 @@
         <f t="shared" si="2"/>
         <v>810</v>
       </c>
-    </row>
-    <row r="28" spans="1:17" ht="15">
+      <c r="T27">
+        <f>J27/D27</f>
+        <v>0.10869565217391304</v>
+      </c>
+      <c r="W27">
+        <f>P27/D27</f>
+        <v>0.37391304347826088</v>
+      </c>
+    </row>
+    <row r="28" spans="1:23" ht="14.4">
       <c r="A28" s="2">
         <v>2005</v>
       </c>
@@ -1645,8 +1828,16 @@
         <f t="shared" si="2"/>
         <v>810</v>
       </c>
-    </row>
-    <row r="29" spans="1:17" ht="15">
+      <c r="T28">
+        <f>J28/D28</f>
+        <v>0.35714285714285715</v>
+      </c>
+      <c r="W28">
+        <f>P28/D28</f>
+        <v>0.31428571428571428</v>
+      </c>
+    </row>
+    <row r="29" spans="1:23" ht="14.4">
       <c r="A29" s="2">
         <v>2006</v>
       </c>
@@ -1695,8 +1886,16 @@
         <f t="shared" si="2"/>
         <v>1110</v>
       </c>
-    </row>
-    <row r="30" spans="1:17" ht="15">
+      <c r="T29">
+        <f>J29/D29</f>
+        <v>0.29411764705882354</v>
+      </c>
+      <c r="W29">
+        <f>P29/D29</f>
+        <v>0.41176470588235292</v>
+      </c>
+    </row>
+    <row r="30" spans="1:23" ht="14.4">
       <c r="A30" s="2">
         <v>2007</v>
       </c>
@@ -1745,8 +1944,16 @@
         <f t="shared" si="2"/>
         <v>820</v>
       </c>
-    </row>
-    <row r="31" spans="1:17" ht="15">
+      <c r="T30">
+        <f>J30/D30</f>
+        <v>0.27500000000000002</v>
+      </c>
+      <c r="W30">
+        <f>P30/D30</f>
+        <v>0.22500000000000001</v>
+      </c>
+    </row>
+    <row r="31" spans="1:23" ht="14.4">
       <c r="A31" s="2">
         <v>2008</v>
       </c>
@@ -1795,8 +2002,16 @@
         <f t="shared" si="2"/>
         <v>1165</v>
       </c>
-    </row>
-    <row r="32" spans="1:17" ht="15">
+      <c r="T31">
+        <f>J31/D31</f>
+        <v>0.26363636363636361</v>
+      </c>
+      <c r="W31">
+        <f>P31/D31</f>
+        <v>0.31818181818181818</v>
+      </c>
+    </row>
+    <row r="32" spans="1:23" ht="14.4">
       <c r="A32" s="2">
         <v>2009</v>
       </c>
@@ -1845,8 +2060,16 @@
         <f t="shared" si="2"/>
         <v>960</v>
       </c>
-    </row>
-    <row r="33" spans="1:17" ht="15">
+      <c r="T32">
+        <f>J32/D32</f>
+        <v>0.35185185185185186</v>
+      </c>
+      <c r="W32">
+        <f>P32/D32</f>
+        <v>0.18518518518518517</v>
+      </c>
+    </row>
+    <row r="33" spans="1:23" ht="14.4">
       <c r="A33" s="2">
         <v>2010</v>
       </c>
@@ -1895,8 +2118,16 @@
         <f t="shared" si="2"/>
         <v>970</v>
       </c>
-    </row>
-    <row r="34" spans="1:17" ht="15">
+      <c r="T33">
+        <f>J33/D33</f>
+        <v>0.35</v>
+      </c>
+      <c r="W33">
+        <f>P33/D33</f>
+        <v>0.23333333333333334</v>
+      </c>
+    </row>
+    <row r="34" spans="1:23" ht="14.4">
       <c r="A34" s="2">
         <v>2011</v>
       </c>
@@ -1945,8 +2176,16 @@
         <f t="shared" si="2"/>
         <v>1235</v>
       </c>
-    </row>
-    <row r="35" spans="1:17" ht="15">
+      <c r="T34">
+        <f>J34/D34</f>
+        <v>0.39344262295081966</v>
+      </c>
+      <c r="W34">
+        <f>P34/D34</f>
+        <v>0.26229508196721313</v>
+      </c>
+    </row>
+    <row r="35" spans="1:23" ht="14.4">
       <c r="A35" s="2">
         <v>2012</v>
       </c>
@@ -1995,8 +2234,16 @@
         <f t="shared" si="2"/>
         <v>1310</v>
       </c>
-    </row>
-    <row r="36" spans="1:17" ht="15">
+      <c r="T35">
+        <f>J35/D35</f>
+        <v>0.56923076923076921</v>
+      </c>
+      <c r="W35">
+        <f>P35/D35</f>
+        <v>0.29230769230769232</v>
+      </c>
+    </row>
+    <row r="36" spans="1:23" ht="14.4">
       <c r="A36" s="3">
         <v>2013</v>
       </c>
@@ -2046,7 +2293,7 @@
         <v>860</v>
       </c>
     </row>
-    <row r="37" spans="1:17" ht="15">
+    <row r="37" spans="1:23" ht="14.4">
       <c r="A37" s="3">
         <v>2014</v>
       </c>
@@ -2095,8 +2342,11 @@
         <f t="shared" si="2"/>
         <v>1150</v>
       </c>
-    </row>
-    <row r="38" spans="1:17" ht="15">
+      <c r="T37" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="38" spans="1:23" ht="14.4">
       <c r="A38" s="3">
         <v>2015</v>
       </c>
@@ -2131,6 +2381,40 @@
       </c>
       <c r="M38" s="8">
         <v>2015</v>
+      </c>
+    </row>
+    <row r="39" spans="1:23">
+      <c r="T39" s="12"/>
+      <c r="W39" s="12"/>
+    </row>
+    <row r="40" spans="1:23">
+      <c r="S40" t="s">
+        <v>10</v>
+      </c>
+      <c r="T40">
+        <f>AVERAGE(T15:T38)</f>
+        <v>0.16822566525857027</v>
+      </c>
+      <c r="V40" t="s">
+        <v>12</v>
+      </c>
+      <c r="W40">
+        <f>AVERAGE(W15:W38) + 1</f>
+        <v>1.3217209210249832</v>
+      </c>
+    </row>
+    <row r="42" spans="1:23">
+      <c r="F42" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="43" spans="1:23">
+      <c r="T43" t="s">
+        <v>14</v>
+      </c>
+      <c r="U43">
+        <f>W40-T40</f>
+        <v>1.1534952557664129</v>
       </c>
     </row>
   </sheetData>
@@ -2140,24 +2424,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultRowHeight="13.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultRowHeight="13.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>